<commit_message>
create api merchants : -> register -> login -> forgot-password -> get single merchant -> edit merchant -> edit picture merchant -> change status merchant (open/close)
</commit_message>
<xml_diff>
--- a/noted/gantt-chart.xlsx
+++ b/noted/gantt-chart.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MagangCrosstechno\e-commerce\noted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD9231E-774E-4781-887D-A932D0DADE88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C9B138-A128-4629-93AE-6CD9E7FF824C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{CDD08313-3D28-49DA-BFCD-6C2CA65C85A7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{CDD08313-3D28-49DA-BFCD-6C2CA65C85A7}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
     <sheet name="test" sheetId="3" r:id="rId2"/>
+    <sheet name="dummy" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="44">
   <si>
     <t>Taks</t>
   </si>
@@ -147,6 +148,24 @@
   </si>
   <si>
     <t>jam 08.00-11.25 (7)</t>
+  </si>
+  <si>
+    <t>jam 11.25 - 14.00 (7)</t>
+  </si>
+  <si>
+    <t>get merchants by products name</t>
+  </si>
+  <si>
+    <t>get merchats by product name</t>
+  </si>
+  <si>
+    <t>edit status merchant</t>
+  </si>
+  <si>
+    <t>jam 14.00 - 16.45 (7)</t>
+  </si>
+  <si>
+    <t>get merchant by product name</t>
   </si>
 </sst>
 </file>
@@ -171,7 +190,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,8 +203,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -254,11 +279,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -295,6 +357,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,17 +689,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3554D58C-1EC2-437D-BF9D-C338C4F56D22}">
-  <dimension ref="A1:S35"/>
+  <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:R36"/>
+      <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22:K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.453125" customWidth="1"/>
-    <col min="2" max="2" width="24.1796875" customWidth="1"/>
+    <col min="2" max="2" width="29.26953125" customWidth="1"/>
     <col min="3" max="18" width="4.6328125" customWidth="1"/>
     <col min="19" max="20" width="8.6328125" customWidth="1"/>
   </cols>
@@ -924,7 +1004,7 @@
       <c r="R12" s="2"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="18" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -948,7 +1028,7 @@
       <c r="R13" s="2"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="9"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="2" t="s">
         <v>8</v>
       </c>
@@ -970,7 +1050,7 @@
       <c r="R14" s="2"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" s="9"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
@@ -995,7 +1075,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" s="9"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="2" t="s">
         <v>10</v>
       </c>
@@ -1017,7 +1097,7 @@
       <c r="R16" s="2"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A17" s="9"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="2" t="s">
         <v>11</v>
       </c>
@@ -1039,7 +1119,7 @@
       <c r="R17" s="2"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A18" s="9"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
@@ -1061,7 +1141,7 @@
       <c r="R18" s="2"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A19" s="9"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="2" t="s">
         <v>7</v>
       </c>
@@ -1083,7 +1163,7 @@
       <c r="R19" s="2"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A20" s="9"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
@@ -1107,7 +1187,7 @@
       <c r="R20" s="2"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A21" s="9"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="2" t="s">
         <v>30</v>
       </c>
@@ -1129,11 +1209,9 @@
       <c r="R21" s="2"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A22" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="A22" s="20"/>
       <c r="B22" s="2" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -1153,9 +1231,11 @@
       <c r="R22" s="2"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A23" s="9"/>
+      <c r="A23" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="B23" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -1177,7 +1257,7 @@
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A24" s="9"/>
       <c r="B24" s="2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -1187,19 +1267,19 @@
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
-      <c r="Q24" s="2"/>
+      <c r="Q24" s="7"/>
       <c r="R24" s="2"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A25" s="9"/>
       <c r="B25" s="2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -1221,7 +1301,924 @@
     <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A26" s="9"/>
       <c r="B26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A27" s="9"/>
+      <c r="B27" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A28" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A29" s="9"/>
+      <c r="B29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A30" s="9"/>
+      <c r="B30" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A31" s="9"/>
+      <c r="B31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A32" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A33" s="9"/>
+      <c r="B33" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A34" s="9"/>
+      <c r="B34" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="5"/>
+      <c r="R34" s="2"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A35" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="17"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="5"/>
+      <c r="R35" s="2"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A36" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="17"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A13:A22"/>
+    <mergeCell ref="A5:A12"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C2:R2"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A34"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E578DE45-B250-43BE-8DBF-313BEAEAEC30}">
+  <dimension ref="A1:U37"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T11" sqref="T11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.453125" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="18" width="4.6328125" customWidth="1"/>
+    <col min="19" max="19" width="21.54296875" customWidth="1"/>
+    <col min="20" max="20" width="22.36328125" customWidth="1"/>
+    <col min="21" max="21" width="22.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="13"/>
+      <c r="S2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1">
+        <v>5</v>
+      </c>
+      <c r="G3" s="1">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1">
+        <v>7</v>
+      </c>
+      <c r="I3" s="1">
+        <v>8</v>
+      </c>
+      <c r="J3" s="1">
+        <v>9</v>
+      </c>
+      <c r="K3" s="1">
+        <v>10</v>
+      </c>
+      <c r="L3" s="1">
+        <v>11</v>
+      </c>
+      <c r="M3" s="1">
+        <v>12</v>
+      </c>
+      <c r="N3" s="1">
+        <v>13</v>
+      </c>
+      <c r="O3" s="1">
+        <v>14</v>
+      </c>
+      <c r="P3" s="1">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>16</v>
+      </c>
+      <c r="R3" s="1">
+        <v>17</v>
+      </c>
+      <c r="S3" s="6"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="2"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="2"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A6" s="9"/>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="2"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A7" s="9"/>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="2"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A8" s="9"/>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="2"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A9" s="9"/>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="2"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A10" s="9"/>
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A11" s="9"/>
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A12" s="9"/>
+      <c r="B12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A13" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="T13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A14" s="19"/>
+      <c r="B14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="T14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A15" s="19"/>
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" t="s">
+        <v>4</v>
+      </c>
+      <c r="T15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A16" s="19"/>
+      <c r="B16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="T16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A17" s="19"/>
+      <c r="B17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="U17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A18" s="19"/>
+      <c r="B18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="U18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A19" s="19"/>
+      <c r="B19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="2"/>
+      <c r="U19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A20" s="19"/>
+      <c r="B20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="2"/>
+      <c r="U20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A21" s="19"/>
+      <c r="B21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="2"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A22" s="19"/>
+      <c r="B22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="2"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A23" s="20"/>
+      <c r="B23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="2"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A24" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="2"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A25" s="9"/>
+      <c r="B25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="2"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A26" s="9"/>
+      <c r="B26" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -1243,12 +2240,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A27" s="9" t="s">
-        <v>21</v>
-      </c>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A27" s="9"/>
       <c r="B27" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -1262,15 +2257,15 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
+      <c r="O27" s="2"/>
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28" s="9"/>
       <c r="B28" s="2" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -1281,18 +2276,20 @@
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="5"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="2"/>
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A29" s="9"/>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A29" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="B29" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -1304,27 +2301,27 @@
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="5"/>
       <c r="O29" s="5"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30" s="9"/>
       <c r="B30" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -1333,34 +2330,32 @@
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A31" s="9" t="s">
-        <v>28</v>
-      </c>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A31" s="9"/>
       <c r="B31" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32" s="9"/>
       <c r="B32" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1374,15 +2369,17 @@
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
-      <c r="P32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A33" s="9"/>
+      <c r="A33" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="B33" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1398,14 +2395,14 @@
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
       <c r="P33" s="5"/>
-      <c r="Q33" s="5"/>
+      <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A34" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="8"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -1419,15 +2416,15 @@
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
-      <c r="Q34" s="5"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A35" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="8"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -1441,45 +2438,91 @@
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
-      <c r="P35" s="2"/>
-      <c r="Q35" s="2"/>
-      <c r="R35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5"/>
+      <c r="R35" s="2"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A36" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="5"/>
+      <c r="R36" s="2"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A37" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="8"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="C2:R2"/>
+    <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:A12"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C2:R2"/>
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A33"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E578DE45-B250-43BE-8DBF-313BEAEAEC30}">
-  <dimension ref="A1:S35"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C37DE0-70AC-4812-9C06-F184D6405EDF}">
+  <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S15" sqref="S15"/>
+      <pane ySplit="3" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.453125" customWidth="1"/>
-    <col min="2" max="2" width="24.1796875" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="18" width="4.6328125" customWidth="1"/>
     <col min="19" max="19" width="21.54296875" customWidth="1"/>
-    <col min="20" max="20" width="8.6328125" customWidth="1"/>
+    <col min="20" max="20" width="22.36328125" customWidth="1"/>
+    <col min="21" max="21" width="22.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1589,7 +2632,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="8"/>
-      <c r="C4" s="5"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="3"/>
@@ -1732,13 +2775,13 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
       <c r="S10" t="s">
         <v>37</v>
       </c>
@@ -1757,13 +2800,13 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
       <c r="S11" t="s">
         <v>37</v>
       </c>
@@ -1782,19 +2825,19 @@
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
       <c r="S12" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="18" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1805,20 +2848,23 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="9"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="2" t="s">
         <v>8</v>
       </c>
@@ -1827,20 +2873,23 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" s="9"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1849,23 +2898,23 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
       <c r="S15" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" s="9"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="2" t="s">
         <v>10</v>
       </c>
@@ -1874,20 +2923,23 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A17" s="9"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="2" t="s">
         <v>11</v>
       </c>
@@ -1896,20 +2948,23 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+      <c r="H17" s="5"/>
       <c r="I17" s="3"/>
-      <c r="J17" s="5"/>
+      <c r="J17" s="3"/>
       <c r="K17" s="3"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A18" s="9"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
@@ -1918,20 +2973,23 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+      <c r="H18" s="5"/>
       <c r="I18" s="3"/>
-      <c r="J18" s="5"/>
+      <c r="J18" s="3"/>
       <c r="K18" s="3"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A19" s="9"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="2" t="s">
         <v>7</v>
       </c>
@@ -1940,20 +2998,23 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+      <c r="H19" s="5"/>
       <c r="I19" s="3"/>
-      <c r="J19" s="5"/>
+      <c r="J19" s="3"/>
       <c r="K19" s="3"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="2"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="3"/>
+      <c r="S19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A20" s="9"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
@@ -1964,46 +3025,50 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+      <c r="H20" s="5"/>
       <c r="I20" s="3"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="2"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="21"/>
+      <c r="R20" s="3"/>
+      <c r="S20" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A21" s="9"/>
-      <c r="B21" s="2" t="s">
-        <v>30</v>
+      <c r="A21" s="19"/>
+      <c r="B21" s="22" t="s">
+        <v>41</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
+      <c r="H21" s="5"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="2"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="21"/>
+      <c r="R21" s="3"/>
+      <c r="S21" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A22" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="A22" s="19"/>
       <c r="B22" s="2" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -2011,21 +3076,21 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
+      <c r="I22" s="23"/>
       <c r="J22" s="3"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="7"/>
-      <c r="R22" s="2"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="21"/>
+      <c r="R22" s="3"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A23" s="9"/>
+      <c r="A23" s="20"/>
       <c r="B23" s="2" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -2033,21 +3098,23 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
+      <c r="I23" s="23"/>
       <c r="J23" s="3"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="7"/>
-      <c r="R23" s="2"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="21"/>
+      <c r="R23" s="3"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A24" s="9"/>
+      <c r="A24" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="B24" s="2" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -2055,21 +3122,21 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
+      <c r="I24" s="5"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="2"/>
-      <c r="R24" s="2"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="21"/>
+      <c r="R24" s="3"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A25" s="9"/>
       <c r="B25" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -2082,16 +3149,16 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="21"/>
+      <c r="R25" s="3"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A26" s="9"/>
       <c r="B26" s="2" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -2104,21 +3171,19 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
-      <c r="N26" s="5"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
-      <c r="Q26" s="2"/>
-      <c r="R26" s="2"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
       <c r="S26" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A27" s="9" t="s">
-        <v>21</v>
-      </c>
+      <c r="A27" s="9"/>
       <c r="B27" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -2131,16 +3196,16 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
-      <c r="P27" s="2"/>
-      <c r="Q27" s="2"/>
-      <c r="R27" s="2"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A28" s="9"/>
       <c r="B28" s="2" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -2151,18 +3216,20 @@
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="5"/>
-      <c r="P28" s="2"/>
-      <c r="Q28" s="2"/>
-      <c r="R28" s="2"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A29" s="9"/>
+      <c r="A29" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="B29" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -2174,162 +3241,205 @@
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="2"/>
-      <c r="Q29" s="2"/>
-      <c r="R29" s="2"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A30" s="9"/>
       <c r="B30" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="5"/>
-      <c r="P30" s="2"/>
-      <c r="Q30" s="2"/>
-      <c r="R30" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A31" s="9" t="s">
-        <v>28</v>
-      </c>
+      <c r="A31" s="9"/>
       <c r="B31" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="5"/>
-      <c r="Q31" s="2"/>
-      <c r="R31" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A32" s="9"/>
       <c r="B32" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
-      <c r="P32" s="5"/>
-      <c r="Q32" s="2"/>
-      <c r="R32" s="2"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A33" s="9"/>
+      <c r="A33" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="B33" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="2"/>
-      <c r="P33" s="5"/>
-      <c r="Q33" s="5"/>
-      <c r="R33" s="2"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A34" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="8"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
-      <c r="Q34" s="5"/>
-      <c r="R34" s="2"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A35" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="8"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
-      <c r="O35" s="2"/>
-      <c r="P35" s="2"/>
-      <c r="Q35" s="2"/>
-      <c r="R35" s="5"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A36" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
+      <c r="R36" s="3"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A37" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="8"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="A2:B3"/>
     <mergeCell ref="C2:R2"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:A12"/>
-    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="A13:A23"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
create api merchants : -> get merchants by product name -> get product merchants create api products : -> add products -> edit products -> get all products -> get product detail -> delete product -> delete product image -> add product image -> edit status product
</commit_message>
<xml_diff>
--- a/noted/gantt-chart.xlsx
+++ b/noted/gantt-chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MagangCrosstechno\e-commerce\noted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C9B138-A128-4629-93AE-6CD9E7FF824C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D4BFBB-F390-4377-BEAD-633E91DA0FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{CDD08313-3D28-49DA-BFCD-6C2CA65C85A7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="49">
   <si>
     <t>Taks</t>
   </si>
@@ -166,6 +166,21 @@
   </si>
   <si>
     <t>get merchant by product name</t>
+  </si>
+  <si>
+    <t>add product image</t>
+  </si>
+  <si>
+    <t>edit status product</t>
+  </si>
+  <si>
+    <t>delete product image</t>
+  </si>
+  <si>
+    <t>jam 08.00 - 13.10 (8)</t>
+  </si>
+  <si>
+    <t>jam 14:05 - 15:00 (8)</t>
   </si>
 </sst>
 </file>
@@ -190,7 +205,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -200,12 +215,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -333,14 +342,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -354,27 +374,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -692,8 +701,8 @@
   <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22:K22"/>
+      <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -705,54 +714,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="13"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="18"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="1">
         <v>2</v>
       </c>
@@ -804,10 +813,10 @@
       <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="5"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -826,7 +835,7 @@
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -850,7 +859,7 @@
       <c r="R5" s="2"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" s="9"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -872,7 +881,7 @@
       <c r="R6" s="2"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A7" s="9"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
@@ -894,7 +903,7 @@
       <c r="R7" s="2"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A8" s="9"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
@@ -916,7 +925,7 @@
       <c r="R8" s="2"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" s="9"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
@@ -938,7 +947,7 @@
       <c r="R9" s="2"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10" s="9"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="2" t="s">
         <v>26</v>
       </c>
@@ -960,7 +969,7 @@
       <c r="R10" s="2"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" s="9"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
@@ -982,7 +991,7 @@
       <c r="R11" s="2"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12" s="9"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="2" t="s">
         <v>27</v>
       </c>
@@ -1004,7 +1013,7 @@
       <c r="R12" s="2"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1028,7 +1037,7 @@
       <c r="R13" s="2"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="19"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="2" t="s">
         <v>8</v>
       </c>
@@ -1050,7 +1059,7 @@
       <c r="R14" s="2"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" s="19"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1075,7 +1084,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" s="19"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="2" t="s">
         <v>10</v>
       </c>
@@ -1097,7 +1106,7 @@
       <c r="R16" s="2"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A17" s="19"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="2" t="s">
         <v>11</v>
       </c>
@@ -1119,7 +1128,7 @@
       <c r="R17" s="2"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A18" s="19"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
@@ -1141,7 +1150,7 @@
       <c r="R18" s="2"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A19" s="19"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="2" t="s">
         <v>7</v>
       </c>
@@ -1163,7 +1172,7 @@
       <c r="R19" s="2"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A20" s="19"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
@@ -1187,7 +1196,7 @@
       <c r="R20" s="2"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A21" s="19"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="2" t="s">
         <v>30</v>
       </c>
@@ -1209,7 +1218,7 @@
       <c r="R21" s="2"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A22" s="20"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="2" t="s">
         <v>39</v>
       </c>
@@ -1231,7 +1240,7 @@
       <c r="R22" s="2"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="13" t="s">
         <v>16</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1255,7 +1264,7 @@
       <c r="R23" s="2"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A24" s="9"/>
+      <c r="A24" s="13"/>
       <c r="B24" s="2" t="s">
         <v>18</v>
       </c>
@@ -1277,7 +1286,7 @@
       <c r="R24" s="2"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A25" s="9"/>
+      <c r="A25" s="13"/>
       <c r="B25" s="2" t="s">
         <v>29</v>
       </c>
@@ -1299,7 +1308,7 @@
       <c r="R25" s="2"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A26" s="9"/>
+      <c r="A26" s="13"/>
       <c r="B26" s="2" t="s">
         <v>19</v>
       </c>
@@ -1321,7 +1330,7 @@
       <c r="R26" s="2"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A27" s="9"/>
+      <c r="A27" s="13"/>
       <c r="B27" s="2" t="s">
         <v>20</v>
       </c>
@@ -1346,7 +1355,7 @@
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="13" t="s">
         <v>21</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -1370,7 +1379,7 @@
       <c r="R28" s="2"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A29" s="9"/>
+      <c r="A29" s="13"/>
       <c r="B29" s="2" t="s">
         <v>35</v>
       </c>
@@ -1392,7 +1401,7 @@
       <c r="R29" s="2"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A30" s="9"/>
+      <c r="A30" s="13"/>
       <c r="B30" s="2" t="s">
         <v>23</v>
       </c>
@@ -1414,7 +1423,7 @@
       <c r="R30" s="2"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A31" s="9"/>
+      <c r="A31" s="13"/>
       <c r="B31" s="2" t="s">
         <v>24</v>
       </c>
@@ -1436,7 +1445,7 @@
       <c r="R31" s="2"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -1460,7 +1469,7 @@
       <c r="R32" s="2"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A33" s="9"/>
+      <c r="A33" s="13"/>
       <c r="B33" s="2" t="s">
         <v>25</v>
       </c>
@@ -1482,7 +1491,7 @@
       <c r="R33" s="2"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A34" s="9"/>
+      <c r="A34" s="13"/>
       <c r="B34" s="2" t="s">
         <v>32</v>
       </c>
@@ -1504,10 +1513,10 @@
       <c r="R34" s="2"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="17"/>
+      <c r="B35" s="21"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -1526,10 +1535,10 @@
       <c r="R35" s="2"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A36" s="16" t="s">
+      <c r="A36" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="17"/>
+      <c r="B36" s="21"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -1549,17 +1558,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A13:A22"/>
-    <mergeCell ref="A5:A12"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C2:R2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A23:A27"/>
     <mergeCell ref="A28:A31"/>
     <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A13:A22"/>
+    <mergeCell ref="A5:A12"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C2:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1571,7 +1580,7 @@
   <dimension ref="A1:U37"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
@@ -1586,57 +1595,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="13"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="18"/>
       <c r="S2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="1">
         <v>2</v>
       </c>
@@ -1688,10 +1697,10 @@
       <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="5"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -1710,7 +1719,7 @@
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1734,7 +1743,7 @@
       <c r="R5" s="2"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A6" s="9"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1756,7 +1765,7 @@
       <c r="R6" s="2"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A7" s="9"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1778,7 +1787,7 @@
       <c r="R7" s="2"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A8" s="9"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1800,7 +1809,7 @@
       <c r="R8" s="2"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A9" s="9"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
@@ -1822,7 +1831,7 @@
       <c r="R9" s="2"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A10" s="9"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="2" t="s">
         <v>26</v>
       </c>
@@ -1847,7 +1856,7 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A11" s="9"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1872,7 +1881,7 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A12" s="9"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="2" t="s">
         <v>27</v>
       </c>
@@ -1897,7 +1906,7 @@
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1924,7 +1933,7 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A14" s="19"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="2" t="s">
         <v>8</v>
       </c>
@@ -1949,7 +1958,7 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A15" s="19"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1977,7 +1986,7 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A16" s="19"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="2" t="s">
         <v>10</v>
       </c>
@@ -2002,7 +2011,7 @@
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A17" s="19"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="2" t="s">
         <v>11</v>
       </c>
@@ -2027,7 +2036,7 @@
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A18" s="19"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
@@ -2052,7 +2061,7 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A19" s="19"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="2" t="s">
         <v>7</v>
       </c>
@@ -2077,7 +2086,7 @@
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A20" s="19"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
@@ -2104,7 +2113,7 @@
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A21" s="19"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="2" t="s">
         <v>30</v>
       </c>
@@ -2126,7 +2135,7 @@
       <c r="R21" s="2"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A22" s="19"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="2" t="s">
         <v>41</v>
       </c>
@@ -2148,7 +2157,7 @@
       <c r="R22" s="2"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A23" s="20"/>
+      <c r="A23" s="12"/>
       <c r="B23" s="2" t="s">
         <v>40</v>
       </c>
@@ -2170,7 +2179,7 @@
       <c r="R23" s="2"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="13" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -2194,7 +2203,7 @@
       <c r="R24" s="2"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A25" s="9"/>
+      <c r="A25" s="13"/>
       <c r="B25" s="2" t="s">
         <v>18</v>
       </c>
@@ -2216,7 +2225,7 @@
       <c r="R25" s="2"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A26" s="9"/>
+      <c r="A26" s="13"/>
       <c r="B26" s="2" t="s">
         <v>29</v>
       </c>
@@ -2241,7 +2250,7 @@
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A27" s="9"/>
+      <c r="A27" s="13"/>
       <c r="B27" s="2" t="s">
         <v>19</v>
       </c>
@@ -2263,7 +2272,7 @@
       <c r="R27" s="2"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A28" s="9"/>
+      <c r="A28" s="13"/>
       <c r="B28" s="2" t="s">
         <v>20</v>
       </c>
@@ -2285,7 +2294,7 @@
       <c r="R28" s="2"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="13" t="s">
         <v>21</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -2309,7 +2318,7 @@
       <c r="R29" s="2"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A30" s="9"/>
+      <c r="A30" s="13"/>
       <c r="B30" s="2" t="s">
         <v>35</v>
       </c>
@@ -2331,7 +2340,7 @@
       <c r="R30" s="2"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A31" s="9"/>
+      <c r="A31" s="13"/>
       <c r="B31" s="2" t="s">
         <v>23</v>
       </c>
@@ -2353,7 +2362,7 @@
       <c r="R31" s="2"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A32" s="9"/>
+      <c r="A32" s="13"/>
       <c r="B32" s="2" t="s">
         <v>24</v>
       </c>
@@ -2375,7 +2384,7 @@
       <c r="R32" s="2"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -2399,7 +2408,7 @@
       <c r="R33" s="2"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A34" s="9"/>
+      <c r="A34" s="13"/>
       <c r="B34" s="2" t="s">
         <v>25</v>
       </c>
@@ -2421,7 +2430,7 @@
       <c r="R34" s="2"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A35" s="9"/>
+      <c r="A35" s="13"/>
       <c r="B35" s="2" t="s">
         <v>32</v>
       </c>
@@ -2443,10 +2452,10 @@
       <c r="R35" s="2"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="8"/>
+      <c r="B36" s="15"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -2465,10 +2474,10 @@
       <c r="R36" s="2"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="8"/>
+      <c r="B37" s="15"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -2488,17 +2497,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
     <mergeCell ref="A13:A23"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="A2:B3"/>
     <mergeCell ref="C2:R2"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:A12"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2508,11 +2517,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C37DE0-70AC-4812-9C06-F184D6405EDF}">
-  <dimension ref="A1:S37"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <pane ySplit="3" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S33" sqref="S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2526,57 +2535,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="13"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="18"/>
       <c r="S2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="1">
         <v>2</v>
       </c>
@@ -2628,10 +2637,10 @@
       <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="3"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -2650,7 +2659,7 @@
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -2674,7 +2683,7 @@
       <c r="R5" s="2"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" s="9"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -2696,7 +2705,7 @@
       <c r="R6" s="2"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A7" s="9"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
@@ -2718,7 +2727,7 @@
       <c r="R7" s="2"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A8" s="9"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
@@ -2740,7 +2749,7 @@
       <c r="R8" s="2"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" s="9"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
@@ -2762,7 +2771,7 @@
       <c r="R9" s="2"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10" s="9"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="2" t="s">
         <v>26</v>
       </c>
@@ -2787,7 +2796,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" s="9"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
@@ -2812,7 +2821,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12" s="9"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="2" t="s">
         <v>27</v>
       </c>
@@ -2837,7 +2846,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -2864,7 +2873,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="19"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="2" t="s">
         <v>8</v>
       </c>
@@ -2889,7 +2898,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" s="19"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
@@ -2914,7 +2923,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" s="19"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="2" t="s">
         <v>10</v>
       </c>
@@ -2939,7 +2948,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A17" s="19"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="2" t="s">
         <v>11</v>
       </c>
@@ -2964,7 +2973,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A18" s="19"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
@@ -2989,7 +2998,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A19" s="19"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="2" t="s">
         <v>7</v>
       </c>
@@ -3007,14 +3016,14 @@
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
-      <c r="Q19" s="21"/>
+      <c r="Q19" s="8"/>
       <c r="R19" s="3"/>
       <c r="S19" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A20" s="19"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
@@ -3034,15 +3043,15 @@
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
-      <c r="Q20" s="21"/>
+      <c r="Q20" s="8"/>
       <c r="R20" s="3"/>
       <c r="S20" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A21" s="19"/>
-      <c r="B21" s="22" t="s">
+      <c r="A21" s="11"/>
+      <c r="B21" s="9" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="3"/>
@@ -3059,14 +3068,14 @@
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
-      <c r="Q21" s="21"/>
+      <c r="Q21" s="8"/>
       <c r="R21" s="3"/>
       <c r="S21" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A22" s="19"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="2" t="s">
         <v>43</v>
       </c>
@@ -3076,7 +3085,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="23"/>
+      <c r="I22" s="5"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
@@ -3084,11 +3093,14 @@
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
-      <c r="Q22" s="21"/>
+      <c r="Q22" s="8"/>
       <c r="R22" s="3"/>
+      <c r="S22" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A23" s="20"/>
+      <c r="A23" s="12"/>
       <c r="B23" s="2" t="s">
         <v>30</v>
       </c>
@@ -3098,7 +3110,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="23"/>
+      <c r="I23" s="5"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
@@ -3106,11 +3118,14 @@
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
-      <c r="Q23" s="21"/>
+      <c r="Q23" s="8"/>
       <c r="R23" s="3"/>
+      <c r="S23" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -3130,13 +3145,16 @@
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
-      <c r="Q24" s="21"/>
+      <c r="Q24" s="8"/>
       <c r="R24" s="3"/>
+      <c r="S24" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A25" s="9"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="2" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -3144,7 +3162,7 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
+      <c r="I25" s="5"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
@@ -3152,13 +3170,16 @@
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
-      <c r="Q25" s="21"/>
+      <c r="Q25" s="8"/>
       <c r="R25" s="3"/>
+      <c r="S25" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A26" s="9"/>
+      <c r="A26" s="11"/>
       <c r="B26" s="2" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -3166,7 +3187,7 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
+      <c r="I26" s="5"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
@@ -3174,16 +3195,16 @@
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
+      <c r="Q26" s="8"/>
       <c r="R26" s="3"/>
       <c r="S26" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A27" s="9"/>
+      <c r="A27" s="11"/>
       <c r="B27" s="2" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -3191,7 +3212,7 @@
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
+      <c r="I27" s="5"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
@@ -3199,13 +3220,16 @@
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
-      <c r="Q27" s="3"/>
+      <c r="Q27" s="8"/>
       <c r="R27" s="3"/>
+      <c r="S27" s="23" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A28" s="9"/>
+      <c r="A28" s="11"/>
       <c r="B28" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -3213,7 +3237,7 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
+      <c r="I28" s="5"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
@@ -3221,15 +3245,16 @@
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
+      <c r="Q28" s="8"/>
       <c r="R28" s="3"/>
+      <c r="S28" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A29" s="9" t="s">
-        <v>21</v>
-      </c>
+      <c r="A29" s="11"/>
       <c r="B29" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -3237,7 +3262,7 @@
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
+      <c r="I29" s="5"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
@@ -3247,11 +3272,14 @@
       <c r="P29" s="3"/>
       <c r="Q29" s="3"/>
       <c r="R29" s="3"/>
+      <c r="S29" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A30" s="9"/>
+      <c r="A30" s="11"/>
       <c r="B30" s="2" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -3259,7 +3287,7 @@
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
+      <c r="I30" s="5"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
@@ -3269,11 +3297,14 @@
       <c r="P30" s="3"/>
       <c r="Q30" s="3"/>
       <c r="R30" s="3"/>
+      <c r="S30" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A31" s="9"/>
+      <c r="A31" s="12"/>
       <c r="B31" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -3281,7 +3312,7 @@
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
+      <c r="I31" s="5"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
@@ -3291,17 +3322,22 @@
       <c r="P31" s="3"/>
       <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
+      <c r="S31" s="23" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A32" s="9"/>
+      <c r="A32" s="13" t="s">
+        <v>21</v>
+      </c>
       <c r="B32" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
@@ -3315,17 +3351,15 @@
       <c r="R32" s="3"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A33" s="9" t="s">
-        <v>28</v>
-      </c>
+      <c r="A33" s="13"/>
       <c r="B33" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
@@ -3339,15 +3373,15 @@
       <c r="R33" s="3"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A34" s="9"/>
+      <c r="A34" s="13"/>
       <c r="B34" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
@@ -3361,9 +3395,9 @@
       <c r="R34" s="3"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A35" s="9"/>
+      <c r="A35" s="13"/>
       <c r="B35" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -3383,10 +3417,12 @@
       <c r="R35" s="3"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A36" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" s="8"/>
+      <c r="A36" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -3405,10 +3441,10 @@
       <c r="R36" s="3"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A37" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B37" s="8"/>
+      <c r="A37" s="13"/>
+      <c r="B37" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -3426,19 +3462,85 @@
       <c r="Q37" s="3"/>
       <c r="R37" s="3"/>
     </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A38" s="13"/>
+      <c r="B38" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="3"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A39" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" s="15"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A40" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" s="15"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="3"/>
+      <c r="R40" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="A24:A31"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="A2:B3"/>
     <mergeCell ref="C2:R2"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:A12"/>
-    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
create api carts -> add product to carts -> get carts -> edit quantity product in carts
</commit_message>
<xml_diff>
--- a/noted/gantt-chart.xlsx
+++ b/noted/gantt-chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MagangCrosstechno\e-commerce\noted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D4BFBB-F390-4377-BEAD-633E91DA0FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E48E03A-5585-446F-87E5-7892F831EE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{CDD08313-3D28-49DA-BFCD-6C2CA65C85A7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="50">
   <si>
     <t>Taks</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>jam 14:05 - 15:00 (8)</t>
+  </si>
+  <si>
+    <t>jam 15.00 - 17.00 (8)</t>
   </si>
 </sst>
 </file>
@@ -2520,8 +2523,8 @@
   <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S33" sqref="S33"/>
+      <pane ySplit="3" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3339,7 +3342,7 @@
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
+      <c r="I32" s="5"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
@@ -3349,8 +3352,11 @@
       <c r="P32" s="3"/>
       <c r="Q32" s="3"/>
       <c r="R32" s="3"/>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A33" s="13"/>
       <c r="B33" s="2" t="s">
         <v>35</v>
@@ -3361,7 +3367,7 @@
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
+      <c r="I33" s="5"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
@@ -3371,8 +3377,11 @@
       <c r="P33" s="3"/>
       <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A34" s="13"/>
       <c r="B34" s="2" t="s">
         <v>23</v>
@@ -3383,7 +3392,7 @@
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
+      <c r="I34" s="5"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
@@ -3393,8 +3402,11 @@
       <c r="P34" s="3"/>
       <c r="Q34" s="3"/>
       <c r="R34" s="3"/>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A35" s="13"/>
       <c r="B35" s="2" t="s">
         <v>24</v>
@@ -3416,7 +3428,7 @@
       <c r="Q35" s="3"/>
       <c r="R35" s="3"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A36" s="13" t="s">
         <v>28</v>
       </c>
@@ -3440,7 +3452,7 @@
       <c r="Q36" s="3"/>
       <c r="R36" s="3"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A37" s="13"/>
       <c r="B37" s="2" t="s">
         <v>25</v>
@@ -3462,7 +3474,7 @@
       <c r="Q37" s="3"/>
       <c r="R37" s="3"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A38" s="13"/>
       <c r="B38" s="2" t="s">
         <v>32</v>
@@ -3484,7 +3496,7 @@
       <c r="Q38" s="3"/>
       <c r="R38" s="3"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A39" s="15" t="s">
         <v>33</v>
       </c>
@@ -3506,7 +3518,7 @@
       <c r="Q39" s="3"/>
       <c r="R39" s="3"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A40" s="15" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
add api delete product from cart add api edit status products in cart add api create order add api change status order
</commit_message>
<xml_diff>
--- a/noted/gantt-chart.xlsx
+++ b/noted/gantt-chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MagangCrosstechno\e-commerce\noted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E48E03A-5585-446F-87E5-7892F831EE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0810F3F3-A573-4985-91F9-7286E138AA39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{CDD08313-3D28-49DA-BFCD-6C2CA65C85A7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="52">
   <si>
     <t>Taks</t>
   </si>
@@ -184,6 +184,12 @@
   </si>
   <si>
     <t>jam 15.00 - 17.00 (8)</t>
+  </si>
+  <si>
+    <t>change status orders</t>
+  </si>
+  <si>
+    <t>jam 08.00 - 15.30 (9)</t>
   </si>
 </sst>
 </file>
@@ -332,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -347,6 +353,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -354,9 +376,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -374,19 +393,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -717,54 +729,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="16" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="18"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="23"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="1">
         <v>2</v>
       </c>
@@ -816,10 +828,10 @@
       <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="5"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -838,7 +850,7 @@
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="15" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -862,7 +874,7 @@
       <c r="R5" s="2"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" s="13"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -884,7 +896,7 @@
       <c r="R6" s="2"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A7" s="13"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
@@ -906,7 +918,7 @@
       <c r="R7" s="2"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A8" s="13"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
@@ -928,7 +940,7 @@
       <c r="R8" s="2"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" s="13"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
@@ -950,7 +962,7 @@
       <c r="R9" s="2"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10" s="13"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="2" t="s">
         <v>26</v>
       </c>
@@ -972,7 +984,7 @@
       <c r="R10" s="2"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" s="13"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
@@ -994,7 +1006,7 @@
       <c r="R11" s="2"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12" s="13"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="2" t="s">
         <v>27</v>
       </c>
@@ -1016,7 +1028,7 @@
       <c r="R12" s="2"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="16" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1040,7 +1052,7 @@
       <c r="R13" s="2"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="11"/>
+      <c r="A14" s="17"/>
       <c r="B14" s="2" t="s">
         <v>8</v>
       </c>
@@ -1062,7 +1074,7 @@
       <c r="R14" s="2"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" s="11"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1087,7 +1099,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" s="11"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="2" t="s">
         <v>10</v>
       </c>
@@ -1109,7 +1121,7 @@
       <c r="R16" s="2"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A17" s="11"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="2" t="s">
         <v>11</v>
       </c>
@@ -1131,7 +1143,7 @@
       <c r="R17" s="2"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A18" s="11"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
@@ -1153,7 +1165,7 @@
       <c r="R18" s="2"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A19" s="11"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="2" t="s">
         <v>7</v>
       </c>
@@ -1175,7 +1187,7 @@
       <c r="R19" s="2"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A20" s="11"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
@@ -1199,7 +1211,7 @@
       <c r="R20" s="2"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A21" s="11"/>
+      <c r="A21" s="17"/>
       <c r="B21" s="2" t="s">
         <v>30</v>
       </c>
@@ -1221,7 +1233,7 @@
       <c r="R21" s="2"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A22" s="12"/>
+      <c r="A22" s="18"/>
       <c r="B22" s="2" t="s">
         <v>39</v>
       </c>
@@ -1243,7 +1255,7 @@
       <c r="R22" s="2"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="15" t="s">
         <v>16</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1267,7 +1279,7 @@
       <c r="R23" s="2"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A24" s="13"/>
+      <c r="A24" s="15"/>
       <c r="B24" s="2" t="s">
         <v>18</v>
       </c>
@@ -1289,7 +1301,7 @@
       <c r="R24" s="2"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A25" s="13"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="2" t="s">
         <v>29</v>
       </c>
@@ -1311,7 +1323,7 @@
       <c r="R25" s="2"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A26" s="13"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="2" t="s">
         <v>19</v>
       </c>
@@ -1333,7 +1345,7 @@
       <c r="R26" s="2"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A27" s="13"/>
+      <c r="A27" s="15"/>
       <c r="B27" s="2" t="s">
         <v>20</v>
       </c>
@@ -1358,7 +1370,7 @@
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -1382,7 +1394,7 @@
       <c r="R28" s="2"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A29" s="13"/>
+      <c r="A29" s="15"/>
       <c r="B29" s="2" t="s">
         <v>35</v>
       </c>
@@ -1404,7 +1416,7 @@
       <c r="R29" s="2"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A30" s="13"/>
+      <c r="A30" s="15"/>
       <c r="B30" s="2" t="s">
         <v>23</v>
       </c>
@@ -1426,7 +1438,7 @@
       <c r="R30" s="2"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A31" s="13"/>
+      <c r="A31" s="15"/>
       <c r="B31" s="2" t="s">
         <v>24</v>
       </c>
@@ -1448,7 +1460,7 @@
       <c r="R31" s="2"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="15" t="s">
         <v>28</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -1472,7 +1484,7 @@
       <c r="R32" s="2"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A33" s="13"/>
+      <c r="A33" s="15"/>
       <c r="B33" s="2" t="s">
         <v>25</v>
       </c>
@@ -1494,7 +1506,7 @@
       <c r="R33" s="2"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A34" s="13"/>
+      <c r="A34" s="15"/>
       <c r="B34" s="2" t="s">
         <v>32</v>
       </c>
@@ -1516,10 +1528,10 @@
       <c r="R34" s="2"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A35" s="20" t="s">
+      <c r="A35" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="21"/>
+      <c r="B35" s="14"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -1538,10 +1550,10 @@
       <c r="R35" s="2"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A36" s="20" t="s">
+      <c r="A36" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="21"/>
+      <c r="B36" s="14"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -1598,57 +1610,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="16" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="18"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="23"/>
       <c r="S2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="1">
         <v>2</v>
       </c>
@@ -1700,10 +1712,10 @@
       <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="5"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -1722,7 +1734,7 @@
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="15" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1746,7 +1758,7 @@
       <c r="R5" s="2"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A6" s="13"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1768,7 +1780,7 @@
       <c r="R6" s="2"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A7" s="13"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1790,7 +1802,7 @@
       <c r="R7" s="2"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A8" s="13"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1812,7 +1824,7 @@
       <c r="R8" s="2"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A9" s="13"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
@@ -1834,7 +1846,7 @@
       <c r="R9" s="2"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A10" s="13"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="2" t="s">
         <v>26</v>
       </c>
@@ -1859,7 +1871,7 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A11" s="13"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1884,7 +1896,7 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A12" s="13"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="2" t="s">
         <v>27</v>
       </c>
@@ -1909,7 +1921,7 @@
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="16" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1936,7 +1948,7 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A14" s="11"/>
+      <c r="A14" s="17"/>
       <c r="B14" s="2" t="s">
         <v>8</v>
       </c>
@@ -1961,7 +1973,7 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A15" s="11"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1989,7 +2001,7 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A16" s="11"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="2" t="s">
         <v>10</v>
       </c>
@@ -2014,7 +2026,7 @@
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A17" s="11"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="2" t="s">
         <v>11</v>
       </c>
@@ -2039,7 +2051,7 @@
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A18" s="11"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
@@ -2064,7 +2076,7 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A19" s="11"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="2" t="s">
         <v>7</v>
       </c>
@@ -2089,7 +2101,7 @@
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A20" s="11"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
@@ -2116,7 +2128,7 @@
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A21" s="11"/>
+      <c r="A21" s="17"/>
       <c r="B21" s="2" t="s">
         <v>30</v>
       </c>
@@ -2138,7 +2150,7 @@
       <c r="R21" s="2"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A22" s="11"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="2" t="s">
         <v>41</v>
       </c>
@@ -2160,7 +2172,7 @@
       <c r="R22" s="2"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A23" s="12"/>
+      <c r="A23" s="18"/>
       <c r="B23" s="2" t="s">
         <v>40</v>
       </c>
@@ -2182,7 +2194,7 @@
       <c r="R23" s="2"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="15" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -2206,7 +2218,7 @@
       <c r="R24" s="2"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A25" s="13"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="2" t="s">
         <v>18</v>
       </c>
@@ -2228,7 +2240,7 @@
       <c r="R25" s="2"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A26" s="13"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="2" t="s">
         <v>29</v>
       </c>
@@ -2253,7 +2265,7 @@
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A27" s="13"/>
+      <c r="A27" s="15"/>
       <c r="B27" s="2" t="s">
         <v>19</v>
       </c>
@@ -2275,7 +2287,7 @@
       <c r="R27" s="2"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A28" s="13"/>
+      <c r="A28" s="15"/>
       <c r="B28" s="2" t="s">
         <v>20</v>
       </c>
@@ -2297,7 +2309,7 @@
       <c r="R28" s="2"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -2321,7 +2333,7 @@
       <c r="R29" s="2"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A30" s="13"/>
+      <c r="A30" s="15"/>
       <c r="B30" s="2" t="s">
         <v>35</v>
       </c>
@@ -2343,7 +2355,7 @@
       <c r="R30" s="2"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A31" s="13"/>
+      <c r="A31" s="15"/>
       <c r="B31" s="2" t="s">
         <v>23</v>
       </c>
@@ -2365,7 +2377,7 @@
       <c r="R31" s="2"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A32" s="13"/>
+      <c r="A32" s="15"/>
       <c r="B32" s="2" t="s">
         <v>24</v>
       </c>
@@ -2387,7 +2399,7 @@
       <c r="R32" s="2"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="15" t="s">
         <v>28</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -2411,7 +2423,7 @@
       <c r="R33" s="2"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A34" s="13"/>
+      <c r="A34" s="15"/>
       <c r="B34" s="2" t="s">
         <v>25</v>
       </c>
@@ -2433,7 +2445,7 @@
       <c r="R34" s="2"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A35" s="13"/>
+      <c r="A35" s="15"/>
       <c r="B35" s="2" t="s">
         <v>32</v>
       </c>
@@ -2455,10 +2467,10 @@
       <c r="R35" s="2"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="15"/>
+      <c r="B36" s="20"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -2477,10 +2489,10 @@
       <c r="R36" s="2"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="15"/>
+      <c r="B37" s="20"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -2500,17 +2512,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
     <mergeCell ref="A13:A23"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="A2:B3"/>
     <mergeCell ref="C2:R2"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:A12"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2520,11 +2532,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C37DE0-70AC-4812-9C06-F184D6405EDF}">
-  <dimension ref="A1:S40"/>
+  <dimension ref="A1:S41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
+      <pane ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2538,57 +2550,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="16" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="18"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="23"/>
       <c r="S2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="1">
         <v>2</v>
       </c>
@@ -2640,10 +2652,10 @@
       <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="3"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -2662,7 +2674,7 @@
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="15" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -2686,7 +2698,7 @@
       <c r="R5" s="2"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" s="13"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -2708,7 +2720,7 @@
       <c r="R6" s="2"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A7" s="13"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
@@ -2730,7 +2742,7 @@
       <c r="R7" s="2"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A8" s="13"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
@@ -2752,7 +2764,7 @@
       <c r="R8" s="2"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" s="13"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
@@ -2774,7 +2786,7 @@
       <c r="R9" s="2"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10" s="13"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="2" t="s">
         <v>26</v>
       </c>
@@ -2799,7 +2811,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" s="13"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
@@ -2824,7 +2836,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12" s="13"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="2" t="s">
         <v>27</v>
       </c>
@@ -2849,7 +2861,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="16" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -2876,7 +2888,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="11"/>
+      <c r="A14" s="17"/>
       <c r="B14" s="2" t="s">
         <v>8</v>
       </c>
@@ -2901,7 +2913,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" s="11"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
@@ -2926,7 +2938,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" s="11"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="2" t="s">
         <v>10</v>
       </c>
@@ -2951,7 +2963,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A17" s="11"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="2" t="s">
         <v>11</v>
       </c>
@@ -2976,7 +2988,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A18" s="11"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
@@ -3001,7 +3013,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A19" s="11"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="2" t="s">
         <v>7</v>
       </c>
@@ -3026,7 +3038,7 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A20" s="11"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
@@ -3053,7 +3065,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A21" s="11"/>
+      <c r="A21" s="17"/>
       <c r="B21" s="9" t="s">
         <v>41</v>
       </c>
@@ -3078,7 +3090,7 @@
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A22" s="11"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="2" t="s">
         <v>43</v>
       </c>
@@ -3103,7 +3115,7 @@
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A23" s="12"/>
+      <c r="A23" s="18"/>
       <c r="B23" s="2" t="s">
         <v>30</v>
       </c>
@@ -3128,7 +3140,7 @@
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -3155,7 +3167,7 @@
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A25" s="11"/>
+      <c r="A25" s="17"/>
       <c r="B25" s="2" t="s">
         <v>46</v>
       </c>
@@ -3180,7 +3192,7 @@
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A26" s="11"/>
+      <c r="A26" s="17"/>
       <c r="B26" s="2" t="s">
         <v>44</v>
       </c>
@@ -3205,7 +3217,7 @@
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A27" s="11"/>
+      <c r="A27" s="17"/>
       <c r="B27" s="2" t="s">
         <v>45</v>
       </c>
@@ -3225,12 +3237,12 @@
       <c r="P27" s="3"/>
       <c r="Q27" s="8"/>
       <c r="R27" s="3"/>
-      <c r="S27" s="23" t="s">
+      <c r="S27" s="11" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A28" s="11"/>
+      <c r="A28" s="17"/>
       <c r="B28" s="2" t="s">
         <v>18</v>
       </c>
@@ -3255,7 +3267,7 @@
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A29" s="11"/>
+      <c r="A29" s="17"/>
       <c r="B29" s="2" t="s">
         <v>29</v>
       </c>
@@ -3280,7 +3292,7 @@
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A30" s="11"/>
+      <c r="A30" s="17"/>
       <c r="B30" s="2" t="s">
         <v>19</v>
       </c>
@@ -3305,7 +3317,7 @@
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A31" s="12"/>
+      <c r="A31" s="18"/>
       <c r="B31" s="2" t="s">
         <v>20</v>
       </c>
@@ -3325,12 +3337,12 @@
       <c r="P31" s="3"/>
       <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
-      <c r="S31" s="23" t="s">
+      <c r="S31" s="11" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -3357,7 +3369,7 @@
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A33" s="13"/>
+      <c r="A33" s="15"/>
       <c r="B33" s="2" t="s">
         <v>35</v>
       </c>
@@ -3382,7 +3394,7 @@
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A34" s="13"/>
+      <c r="A34" s="15"/>
       <c r="B34" s="2" t="s">
         <v>23</v>
       </c>
@@ -3407,7 +3419,7 @@
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A35" s="13"/>
+      <c r="A35" s="15"/>
       <c r="B35" s="2" t="s">
         <v>24</v>
       </c>
@@ -3418,7 +3430,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
+      <c r="J35" s="5"/>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
@@ -3427,11 +3439,12 @@
       <c r="P35" s="3"/>
       <c r="Q35" s="3"/>
       <c r="R35" s="3"/>
+      <c r="S35" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A36" s="13" t="s">
-        <v>28</v>
-      </c>
+      <c r="A36" s="10"/>
       <c r="B36" s="2" t="s">
         <v>31</v>
       </c>
@@ -3442,7 +3455,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
+      <c r="J36" s="5"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
@@ -3451,11 +3464,16 @@
       <c r="P36" s="3"/>
       <c r="Q36" s="3"/>
       <c r="R36" s="3"/>
+      <c r="S36" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A37" s="13"/>
+      <c r="A37" s="25" t="s">
+        <v>28</v>
+      </c>
       <c r="B37" s="2" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -3464,7 +3482,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
+      <c r="J37" s="5"/>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
@@ -3473,11 +3491,14 @@
       <c r="P37" s="3"/>
       <c r="Q37" s="3"/>
       <c r="R37" s="3"/>
+      <c r="S37" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A38" s="13"/>
+      <c r="A38" s="25"/>
       <c r="B38" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -3486,7 +3507,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
+      <c r="J38" s="5"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
@@ -3495,12 +3516,15 @@
       <c r="P38" s="3"/>
       <c r="Q38" s="3"/>
       <c r="R38" s="3"/>
+      <c r="S38" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A39" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B39" s="15"/>
+      <c r="A39" s="25"/>
+      <c r="B39" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -3508,7 +3532,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
+      <c r="J39" s="5"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
@@ -3517,12 +3541,15 @@
       <c r="P39" s="3"/>
       <c r="Q39" s="3"/>
       <c r="R39" s="3"/>
+      <c r="S39" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A40" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B40" s="15"/>
+      <c r="A40" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" s="20"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -3540,8 +3567,33 @@
       <c r="Q40" s="3"/>
       <c r="R40" s="3"/>
     </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A41" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="20"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="10">
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
     <mergeCell ref="A13:A23"/>
     <mergeCell ref="A24:A31"/>
     <mergeCell ref="A1:R1"/>
@@ -3549,10 +3601,6 @@
     <mergeCell ref="C2:R2"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:A12"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>